<commit_message>
Added links to the files into the files
</commit_message>
<xml_diff>
--- a/German/Modeling-Workshop/Kontensalden.xlsx
+++ b/German/Modeling-Workshop/Kontensalden.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinBubenheimer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE94B3D-0EB3-4EAA-9D48-16EF143173CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4726F4BD-9C7D-4147-A9E0-AC7C60C22C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40710" yWindow="2085" windowWidth="28800" windowHeight="11700" xr2:uid="{3AF09E0F-002F-4D5D-8476-F99A6C04A2A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Kontobewegungen" sheetId="2" r:id="rId1"/>
-    <sheet name="Mehrere Konten" sheetId="4" r:id="rId2"/>
-    <sheet name="Kalender" sheetId="3" r:id="rId3"/>
-    <sheet name="Rechenblatt" sheetId="1" r:id="rId4"/>
+    <sheet name="Link" sheetId="5" r:id="rId1"/>
+    <sheet name="Kontobewegungen" sheetId="2" r:id="rId2"/>
+    <sheet name="Mehrere Konten" sheetId="4" r:id="rId3"/>
+    <sheet name="Kalender" sheetId="3" r:id="rId4"/>
+    <sheet name="Rechenblatt" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="62">
   <si>
     <t>Konto</t>
   </si>
@@ -220,15 +221,29 @@
   <si>
     <t>2023-12</t>
   </si>
+  <si>
+    <t>https://t.ly/IRIpW</t>
+  </si>
+  <si>
+    <t>https://github.com/MartinBubenheimer/powerbi-training/tree/main/German/Modeling-Workshop</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,14 +266,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -282,6 +300,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>45566</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03157C5A-78D5-DFFA-0C12-133FF42029E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="180975"/>
+          <a:ext cx="3305175" cy="3303116"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,11 +701,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B547A9F7-9E32-4D87-8987-D2DAB6A44C87}">
+  <dimension ref="B21:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{549A66BC-9B8A-42DC-988B-44B16EC3F46D}"/>
+    <hyperlink ref="B23" r:id="rId2" xr:uid="{813D180D-5B39-4E5E-8342-26D27F50A929}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8595DE23-8F51-44D3-94EA-77712C9EA1B3}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="A1:F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -883,7 +989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43AC6B2F-F680-4823-8889-56F9C650350F}">
   <dimension ref="A1:F27"/>
   <sheetViews>
@@ -1360,7 +1466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19D5C18-2A65-4206-A837-E75189DFE989}">
   <dimension ref="A1:F731"/>
   <sheetViews>
@@ -16006,7 +16112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AB3D30-38D5-4442-851A-46F4479B6B9D}">
   <dimension ref="A1:F14"/>
   <sheetViews>

</xml_diff>